<commit_message>
add rob to publications
</commit_message>
<xml_diff>
--- a/analysis/data_commit/delete_list.xlsx
+++ b/analysis/data_commit/delete_list.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9856AC31-3259-48B8-A586-CF2C680479CE}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/dev/marks/2024/cpvt_database_analysis/analysis/data_commit/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0B8384-E749-F94B-A056-7E07C632B0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="30960" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>publication_id</t>
   </si>
@@ -109,13 +114,31 @@
   </si>
   <si>
     <t>No specific RYR2 mutation mentioned</t>
+  </si>
+  <si>
+    <t>Fatal arrhythmias associated with genetic variants in type 2 ryanodine receptor channel gene</t>
+  </si>
+  <si>
+    <t>Novel mutations in arrhythmogenic right ventricular cardiomyopathy from Indian population</t>
+  </si>
+  <si>
+    <t>Horie, M.</t>
+  </si>
+  <si>
+    <t>Pamuru, PR</t>
+  </si>
+  <si>
+    <t>10.1007/s10840-018-0338-y</t>
+  </si>
+  <si>
+    <t>10.4103/0971-6866.86182</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,11 +156,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -183,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -191,6 +215,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M15" sqref="M15:M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -556,7 +581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>827</v>
       </c>
@@ -579,7 +604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1096</v>
       </c>
@@ -602,7 +627,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>690</v>
       </c>
@@ -620,7 +645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>406</v>
       </c>
@@ -636,6 +661,34 @@
       </c>
       <c r="G5" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>1343</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX ERROR: analyze patient demographics by counting patient ids UNIQUE
</commit_message>
<xml_diff>
--- a/analysis/data_commit/delete_list.xlsx
+++ b/analysis/data_commit/delete_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/dev/marks/2024/cpvt_database_analysis/analysis/data_commit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0B8384-E749-F94B-A056-7E07C632B0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84A7970-D0F2-0748-88BC-6395832D53C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="30960" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>publication_id</t>
   </si>
@@ -53,9 +53,6 @@
     <t>resource_uri</t>
   </si>
   <si>
-    <t>doi_hyperlink</t>
-  </si>
-  <si>
     <t>delete_reason</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>https://doi.org/10.1016/j.rccar.2019.09.008</t>
-  </si>
-  <si>
     <t>Not in English</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
   </si>
   <si>
     <t>https://www.embase.com/records?id=L354806040</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.2174/1875692110806030185</t>
   </si>
   <si>
     <t>Cannot access article</t>
@@ -166,18 +157,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -209,13 +194,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,145 +535,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15:M16"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>827</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>827</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1096</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>1096</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>690</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>690</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>406</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
-        <v>18</v>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>406</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>121</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1343</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>121</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>1343</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>